<commit_message>
Updated with Andy's feedback
</commit_message>
<xml_diff>
--- a/Pin mapping/core-pin-mapping.xlsx
+++ b/Pin mapping/core-pin-mapping.xlsx
@@ -1140,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1491,6 +1491,9 @@
       <c r="K12">
         <v>31</v>
       </c>
+      <c r="L12" s="4" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="3" t="s">
@@ -1935,9 +1938,6 @@
       </c>
       <c r="K29">
         <v>22</v>
-      </c>
-      <c r="L29" s="4" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -2209,7 +2209,7 @@
         <v>9</v>
       </c>
       <c r="L43" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2321,7 +2321,7 @@
   <dimension ref="B1:M28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3195,7 +3195,7 @@
         <v>22</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>

</xml_diff>

<commit_message>
Finished Core Debug v0.0.8
</commit_message>
<xml_diff>
--- a/Pin mapping/core-pin-mapping.xlsx
+++ b/Pin mapping/core-pin-mapping.xlsx
@@ -1140,8 +1140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1862,6 +1862,9 @@
       <c r="K26">
         <v>45</v>
       </c>
+      <c r="L26" s="4" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="3" t="s">
@@ -1938,6 +1941,9 @@
       </c>
       <c r="K29">
         <v>22</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -2072,9 +2078,6 @@
       <c r="K34">
         <v>2</v>
       </c>
-      <c r="L34" s="4" t="s">
-        <v>178</v>
-      </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="3" t="s">
@@ -2093,9 +2096,6 @@
       </c>
       <c r="K35">
         <v>3</v>
-      </c>
-      <c r="L35" s="4" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:12">

</xml_diff>